<commit_message>
Another Mini Fix before staging
</commit_message>
<xml_diff>
--- a/billing/Prod/rates/rates.xlsx
+++ b/billing/Prod/rates/rates.xlsx
@@ -162,35 +162,35 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -198,10 +198,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -209,10 +209,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -220,10 +220,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -231,10 +231,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -242,10 +242,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -253,10 +253,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -270,7 +270,7 @@
       <c r="B10" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>43</v>
       </c>
     </row>
@@ -281,7 +281,7 @@
       <c r="B11" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>45</v>
       </c>
     </row>
@@ -292,7 +292,7 @@
       <c r="B12" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>12</v>
       </c>
     </row>
@@ -303,7 +303,7 @@
       <c r="B13" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>45</v>
       </c>
     </row>

</xml_diff>